<commit_message>
added ".org" to emulator code
added ".org" to emulator code and updated code to use labels and .org
</commit_message>
<xml_diff>
--- a/Display 16x16/Code/StartCodeAndmemoryMapForGoL.xlsx
+++ b/Display 16x16/Code/StartCodeAndmemoryMapForGoL.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\DCJ11Hack-\Display 16x16\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45D78AA8-34C9-4873-BD38-496A089DFD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9C90A5-E72D-48A7-B502-AD5F8C0AEDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B3B472E-8BB3-40FA-B156-128F36A2A6CF}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{2B3B472E-8BB3-40FA-B156-128F36A2A6CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -474,17 +473,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B525301-A21F-42E0-A7F9-F61494105302}">
   <dimension ref="A1:AY27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16" width="4.125" customWidth="1"/>
-    <col min="19" max="19" width="11.5" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="2.875" hidden="1" customWidth="1"/>
-    <col min="21" max="34" width="3.875" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="0" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" customWidth="1"/>
+    <col min="20" max="20" width="2.875" customWidth="1"/>
+    <col min="21" max="34" width="3.875" customWidth="1"/>
+    <col min="35" max="35" width="9" customWidth="1"/>
     <col min="36" max="36" width="10" style="4" bestFit="1" customWidth="1"/>
     <col min="37" max="51" width="6.875" bestFit="1" customWidth="1"/>
   </cols>
@@ -517,131 +516,131 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="S2">
-        <v>8</v>
+        <v>576</v>
       </c>
       <c r="T2">
         <f t="shared" ref="T2:AH2" si="0">S17+2</f>
-        <v>40</v>
+        <v>608</v>
       </c>
       <c r="U2">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>640</v>
       </c>
       <c r="V2">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>672</v>
       </c>
       <c r="W2">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>704</v>
       </c>
       <c r="X2">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>736</v>
       </c>
       <c r="Y2">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>768</v>
       </c>
       <c r="Z2">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>800</v>
       </c>
       <c r="AA2">
         <f t="shared" si="0"/>
-        <v>264</v>
+        <v>832</v>
       </c>
       <c r="AB2">
         <f t="shared" si="0"/>
-        <v>296</v>
+        <v>864</v>
       </c>
       <c r="AC2">
         <f t="shared" si="0"/>
-        <v>328</v>
+        <v>896</v>
       </c>
       <c r="AD2">
         <f t="shared" si="0"/>
-        <v>360</v>
+        <v>928</v>
       </c>
       <c r="AE2">
         <f t="shared" si="0"/>
-        <v>392</v>
+        <v>960</v>
       </c>
       <c r="AF2">
         <f t="shared" si="0"/>
-        <v>424</v>
+        <v>992</v>
       </c>
       <c r="AG2">
         <f t="shared" si="0"/>
-        <v>456</v>
+        <v>1024</v>
       </c>
       <c r="AH2">
         <f t="shared" si="0"/>
-        <v>488</v>
+        <v>1056</v>
       </c>
       <c r="AJ2" s="4" t="str">
         <f t="shared" ref="AJ2:AL3" si="1">DEC2OCT(S2,6)</f>
-        <v>000010</v>
+        <v>001100</v>
       </c>
       <c r="AK2" t="str">
         <f t="shared" si="1"/>
-        <v>000050</v>
+        <v>001140</v>
       </c>
       <c r="AL2" t="str">
         <f t="shared" si="1"/>
-        <v>000110</v>
+        <v>001200</v>
       </c>
       <c r="AM2" t="str">
         <f t="shared" ref="AM2:AY17" si="2">DEC2OCT(V2,6)</f>
-        <v>000150</v>
+        <v>001240</v>
       </c>
       <c r="AN2" t="str">
         <f t="shared" si="2"/>
-        <v>000210</v>
+        <v>001300</v>
       </c>
       <c r="AO2" t="str">
         <f t="shared" si="2"/>
-        <v>000250</v>
+        <v>001340</v>
       </c>
       <c r="AP2" t="str">
         <f t="shared" si="2"/>
-        <v>000310</v>
+        <v>001400</v>
       </c>
       <c r="AQ2" t="str">
         <f t="shared" si="2"/>
-        <v>000350</v>
+        <v>001440</v>
       </c>
       <c r="AR2" t="str">
         <f t="shared" si="2"/>
-        <v>000410</v>
+        <v>001500</v>
       </c>
       <c r="AS2" t="str">
         <f t="shared" si="2"/>
-        <v>000450</v>
+        <v>001540</v>
       </c>
       <c r="AT2" t="str">
         <f t="shared" si="2"/>
-        <v>000510</v>
+        <v>001600</v>
       </c>
       <c r="AU2" t="str">
         <f t="shared" si="2"/>
-        <v>000550</v>
+        <v>001640</v>
       </c>
       <c r="AV2" t="str">
         <f t="shared" si="2"/>
-        <v>000610</v>
+        <v>001700</v>
       </c>
       <c r="AW2" t="str">
         <f t="shared" si="2"/>
-        <v>000650</v>
+        <v>001740</v>
       </c>
       <c r="AX2" t="str">
         <f t="shared" si="2"/>
-        <v>000710</v>
+        <v>002000</v>
       </c>
       <c r="AY2" t="str">
         <f t="shared" si="2"/>
-        <v>000750</v>
+        <v>002040</v>
       </c>
     </row>
     <row r="3" spans="1:51" ht="24" customHeight="1">
@@ -671,131 +670,131 @@
       <c r="P3" s="1"/>
       <c r="S3">
         <f t="shared" ref="S3:S17" si="3">S2+2</f>
-        <v>10</v>
+        <v>578</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T17" si="4">T2+2</f>
-        <v>42</v>
+        <v>610</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U17" si="5">U2+2</f>
-        <v>74</v>
+        <v>642</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V17" si="6">V2+2</f>
-        <v>106</v>
+        <v>674</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W17" si="7">W2+2</f>
-        <v>138</v>
+        <v>706</v>
       </c>
       <c r="X3">
         <f t="shared" ref="X3:X17" si="8">X2+2</f>
-        <v>170</v>
+        <v>738</v>
       </c>
       <c r="Y3">
         <f t="shared" ref="Y3:Y17" si="9">Y2+2</f>
-        <v>202</v>
+        <v>770</v>
       </c>
       <c r="Z3">
         <f t="shared" ref="Z3:Z17" si="10">Z2+2</f>
-        <v>234</v>
+        <v>802</v>
       </c>
       <c r="AA3">
         <f t="shared" ref="AA3:AA17" si="11">AA2+2</f>
-        <v>266</v>
+        <v>834</v>
       </c>
       <c r="AB3">
         <f t="shared" ref="AB3:AB17" si="12">AB2+2</f>
-        <v>298</v>
+        <v>866</v>
       </c>
       <c r="AC3">
         <f t="shared" ref="AC3:AC17" si="13">AC2+2</f>
-        <v>330</v>
+        <v>898</v>
       </c>
       <c r="AD3">
         <f t="shared" ref="AD3:AD17" si="14">AD2+2</f>
-        <v>362</v>
+        <v>930</v>
       </c>
       <c r="AE3">
         <f t="shared" ref="AE3:AE17" si="15">AE2+2</f>
-        <v>394</v>
+        <v>962</v>
       </c>
       <c r="AF3">
         <f t="shared" ref="AF3:AF17" si="16">AF2+2</f>
-        <v>426</v>
+        <v>994</v>
       </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG17" si="17">AG2+2</f>
-        <v>458</v>
+        <v>1026</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH17" si="18">AH2+2</f>
-        <v>490</v>
+        <v>1058</v>
       </c>
       <c r="AJ3" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>000012</v>
+        <v>001102</v>
       </c>
       <c r="AK3" t="str">
         <f t="shared" si="1"/>
-        <v>000052</v>
+        <v>001142</v>
       </c>
       <c r="AL3" t="str">
         <f t="shared" si="1"/>
-        <v>000112</v>
+        <v>001202</v>
       </c>
       <c r="AM3" t="str">
         <f t="shared" si="2"/>
-        <v>000152</v>
+        <v>001242</v>
       </c>
       <c r="AN3" t="str">
         <f t="shared" si="2"/>
-        <v>000212</v>
+        <v>001302</v>
       </c>
       <c r="AO3" t="str">
         <f t="shared" si="2"/>
-        <v>000252</v>
+        <v>001342</v>
       </c>
       <c r="AP3" t="str">
         <f t="shared" si="2"/>
-        <v>000312</v>
+        <v>001402</v>
       </c>
       <c r="AQ3" t="str">
         <f t="shared" si="2"/>
-        <v>000352</v>
+        <v>001442</v>
       </c>
       <c r="AR3" t="str">
         <f t="shared" si="2"/>
-        <v>000412</v>
+        <v>001502</v>
       </c>
       <c r="AS3" t="str">
         <f t="shared" si="2"/>
-        <v>000452</v>
+        <v>001542</v>
       </c>
       <c r="AT3" t="str">
         <f t="shared" si="2"/>
-        <v>000512</v>
+        <v>001602</v>
       </c>
       <c r="AU3" t="str">
         <f t="shared" si="2"/>
-        <v>000552</v>
+        <v>001642</v>
       </c>
       <c r="AV3" t="str">
         <f t="shared" si="2"/>
-        <v>000612</v>
+        <v>001702</v>
       </c>
       <c r="AW3" t="str">
         <f t="shared" si="2"/>
-        <v>000652</v>
+        <v>001742</v>
       </c>
       <c r="AX3" t="str">
         <f t="shared" si="2"/>
-        <v>000712</v>
+        <v>002002</v>
       </c>
       <c r="AY3" t="str">
         <f t="shared" si="2"/>
-        <v>000752</v>
+        <v>002042</v>
       </c>
     </row>
     <row r="4" spans="1:51" ht="24" customHeight="1">
@@ -823,131 +822,131 @@
       <c r="P4" s="1"/>
       <c r="S4">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>580</v>
       </c>
       <c r="T4">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>612</v>
       </c>
       <c r="U4">
         <f t="shared" si="5"/>
-        <v>76</v>
+        <v>644</v>
       </c>
       <c r="V4">
         <f t="shared" si="6"/>
-        <v>108</v>
+        <v>676</v>
       </c>
       <c r="W4">
         <f t="shared" si="7"/>
-        <v>140</v>
+        <v>708</v>
       </c>
       <c r="X4">
         <f t="shared" si="8"/>
-        <v>172</v>
+        <v>740</v>
       </c>
       <c r="Y4">
         <f t="shared" si="9"/>
-        <v>204</v>
+        <v>772</v>
       </c>
       <c r="Z4">
         <f t="shared" si="10"/>
-        <v>236</v>
+        <v>804</v>
       </c>
       <c r="AA4">
         <f t="shared" si="11"/>
-        <v>268</v>
+        <v>836</v>
       </c>
       <c r="AB4">
         <f t="shared" si="12"/>
-        <v>300</v>
+        <v>868</v>
       </c>
       <c r="AC4">
         <f t="shared" si="13"/>
-        <v>332</v>
+        <v>900</v>
       </c>
       <c r="AD4">
         <f t="shared" si="14"/>
-        <v>364</v>
+        <v>932</v>
       </c>
       <c r="AE4">
         <f t="shared" si="15"/>
-        <v>396</v>
+        <v>964</v>
       </c>
       <c r="AF4">
         <f t="shared" si="16"/>
-        <v>428</v>
+        <v>996</v>
       </c>
       <c r="AG4">
         <f t="shared" si="17"/>
-        <v>460</v>
+        <v>1028</v>
       </c>
       <c r="AH4">
         <f t="shared" si="18"/>
-        <v>492</v>
+        <v>1060</v>
       </c>
       <c r="AJ4" s="4" t="str">
         <f t="shared" ref="AJ4:AL17" si="19">DEC2OCT(S4,6)</f>
-        <v>000014</v>
+        <v>001104</v>
       </c>
       <c r="AK4" t="str">
         <f t="shared" si="19"/>
-        <v>000054</v>
+        <v>001144</v>
       </c>
       <c r="AL4" t="str">
         <f t="shared" si="19"/>
-        <v>000114</v>
+        <v>001204</v>
       </c>
       <c r="AM4" t="str">
         <f t="shared" si="2"/>
-        <v>000154</v>
+        <v>001244</v>
       </c>
       <c r="AN4" t="str">
         <f t="shared" si="2"/>
-        <v>000214</v>
+        <v>001304</v>
       </c>
       <c r="AO4" t="str">
         <f t="shared" si="2"/>
-        <v>000254</v>
+        <v>001344</v>
       </c>
       <c r="AP4" t="str">
         <f t="shared" si="2"/>
-        <v>000314</v>
+        <v>001404</v>
       </c>
       <c r="AQ4" t="str">
         <f t="shared" si="2"/>
-        <v>000354</v>
+        <v>001444</v>
       </c>
       <c r="AR4" t="str">
         <f t="shared" si="2"/>
-        <v>000414</v>
+        <v>001504</v>
       </c>
       <c r="AS4" t="str">
         <f t="shared" si="2"/>
-        <v>000454</v>
+        <v>001544</v>
       </c>
       <c r="AT4" t="str">
         <f t="shared" si="2"/>
-        <v>000514</v>
+        <v>001604</v>
       </c>
       <c r="AU4" t="str">
         <f t="shared" si="2"/>
-        <v>000554</v>
+        <v>001644</v>
       </c>
       <c r="AV4" t="str">
         <f t="shared" si="2"/>
-        <v>000614</v>
+        <v>001704</v>
       </c>
       <c r="AW4" t="str">
         <f t="shared" si="2"/>
-        <v>000654</v>
+        <v>001744</v>
       </c>
       <c r="AX4" t="str">
         <f t="shared" si="2"/>
-        <v>000714</v>
+        <v>002004</v>
       </c>
       <c r="AY4" t="str">
         <f t="shared" si="2"/>
-        <v>000754</v>
+        <v>002044</v>
       </c>
     </row>
     <row r="5" spans="1:51" ht="24" customHeight="1">
@@ -979,131 +978,131 @@
       <c r="P5" s="1"/>
       <c r="S5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>582</v>
       </c>
       <c r="T5">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>614</v>
       </c>
       <c r="U5">
         <f t="shared" si="5"/>
-        <v>78</v>
+        <v>646</v>
       </c>
       <c r="V5">
         <f t="shared" si="6"/>
-        <v>110</v>
+        <v>678</v>
       </c>
       <c r="W5">
         <f t="shared" si="7"/>
-        <v>142</v>
+        <v>710</v>
       </c>
       <c r="X5">
         <f t="shared" si="8"/>
-        <v>174</v>
+        <v>742</v>
       </c>
       <c r="Y5">
         <f t="shared" si="9"/>
-        <v>206</v>
+        <v>774</v>
       </c>
       <c r="Z5">
         <f t="shared" si="10"/>
-        <v>238</v>
+        <v>806</v>
       </c>
       <c r="AA5">
         <f t="shared" si="11"/>
-        <v>270</v>
+        <v>838</v>
       </c>
       <c r="AB5">
         <f t="shared" si="12"/>
-        <v>302</v>
+        <v>870</v>
       </c>
       <c r="AC5">
         <f t="shared" si="13"/>
-        <v>334</v>
+        <v>902</v>
       </c>
       <c r="AD5">
         <f t="shared" si="14"/>
-        <v>366</v>
+        <v>934</v>
       </c>
       <c r="AE5">
         <f t="shared" si="15"/>
-        <v>398</v>
+        <v>966</v>
       </c>
       <c r="AF5">
         <f t="shared" si="16"/>
-        <v>430</v>
+        <v>998</v>
       </c>
       <c r="AG5">
         <f t="shared" si="17"/>
-        <v>462</v>
+        <v>1030</v>
       </c>
       <c r="AH5">
         <f t="shared" si="18"/>
-        <v>494</v>
+        <v>1062</v>
       </c>
       <c r="AJ5" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000016</v>
+        <v>001106</v>
       </c>
       <c r="AK5" t="str">
         <f t="shared" si="19"/>
-        <v>000056</v>
+        <v>001146</v>
       </c>
       <c r="AL5" t="str">
         <f t="shared" si="19"/>
-        <v>000116</v>
+        <v>001206</v>
       </c>
       <c r="AM5" t="str">
         <f t="shared" si="2"/>
-        <v>000156</v>
+        <v>001246</v>
       </c>
       <c r="AN5" t="str">
         <f t="shared" si="2"/>
-        <v>000216</v>
+        <v>001306</v>
       </c>
       <c r="AO5" t="str">
         <f t="shared" si="2"/>
-        <v>000256</v>
+        <v>001346</v>
       </c>
       <c r="AP5" t="str">
         <f t="shared" si="2"/>
-        <v>000316</v>
+        <v>001406</v>
       </c>
       <c r="AQ5" t="str">
         <f t="shared" si="2"/>
-        <v>000356</v>
+        <v>001446</v>
       </c>
       <c r="AR5" t="str">
         <f t="shared" si="2"/>
-        <v>000416</v>
+        <v>001506</v>
       </c>
       <c r="AS5" t="str">
         <f t="shared" si="2"/>
-        <v>000456</v>
+        <v>001546</v>
       </c>
       <c r="AT5" t="str">
         <f t="shared" si="2"/>
-        <v>000516</v>
+        <v>001606</v>
       </c>
       <c r="AU5" t="str">
         <f t="shared" si="2"/>
-        <v>000556</v>
+        <v>001646</v>
       </c>
       <c r="AV5" t="str">
         <f t="shared" si="2"/>
-        <v>000616</v>
+        <v>001706</v>
       </c>
       <c r="AW5" t="str">
         <f t="shared" si="2"/>
-        <v>000656</v>
+        <v>001746</v>
       </c>
       <c r="AX5" t="str">
         <f t="shared" si="2"/>
-        <v>000716</v>
+        <v>002006</v>
       </c>
       <c r="AY5" t="str">
         <f t="shared" si="2"/>
-        <v>000756</v>
+        <v>002046</v>
       </c>
     </row>
     <row r="6" spans="1:51" ht="24" customHeight="1">
@@ -1129,131 +1128,131 @@
       <c r="P6" s="1"/>
       <c r="S6">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>584</v>
       </c>
       <c r="T6">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>616</v>
       </c>
       <c r="U6">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>648</v>
       </c>
       <c r="V6">
         <f t="shared" si="6"/>
-        <v>112</v>
+        <v>680</v>
       </c>
       <c r="W6">
         <f t="shared" si="7"/>
-        <v>144</v>
+        <v>712</v>
       </c>
       <c r="X6">
         <f t="shared" si="8"/>
-        <v>176</v>
+        <v>744</v>
       </c>
       <c r="Y6">
         <f t="shared" si="9"/>
-        <v>208</v>
+        <v>776</v>
       </c>
       <c r="Z6">
         <f t="shared" si="10"/>
-        <v>240</v>
+        <v>808</v>
       </c>
       <c r="AA6">
         <f t="shared" si="11"/>
-        <v>272</v>
+        <v>840</v>
       </c>
       <c r="AB6">
         <f t="shared" si="12"/>
-        <v>304</v>
+        <v>872</v>
       </c>
       <c r="AC6">
         <f t="shared" si="13"/>
-        <v>336</v>
+        <v>904</v>
       </c>
       <c r="AD6">
         <f t="shared" si="14"/>
-        <v>368</v>
+        <v>936</v>
       </c>
       <c r="AE6">
         <f t="shared" si="15"/>
-        <v>400</v>
+        <v>968</v>
       </c>
       <c r="AF6">
         <f t="shared" si="16"/>
-        <v>432</v>
+        <v>1000</v>
       </c>
       <c r="AG6">
         <f t="shared" si="17"/>
-        <v>464</v>
+        <v>1032</v>
       </c>
       <c r="AH6">
         <f t="shared" si="18"/>
-        <v>496</v>
+        <v>1064</v>
       </c>
       <c r="AJ6" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000020</v>
+        <v>001110</v>
       </c>
       <c r="AK6" t="str">
         <f t="shared" si="19"/>
-        <v>000060</v>
+        <v>001150</v>
       </c>
       <c r="AL6" t="str">
         <f t="shared" si="19"/>
-        <v>000120</v>
+        <v>001210</v>
       </c>
       <c r="AM6" t="str">
         <f t="shared" si="2"/>
-        <v>000160</v>
+        <v>001250</v>
       </c>
       <c r="AN6" t="str">
         <f t="shared" si="2"/>
-        <v>000220</v>
+        <v>001310</v>
       </c>
       <c r="AO6" t="str">
         <f t="shared" si="2"/>
-        <v>000260</v>
+        <v>001350</v>
       </c>
       <c r="AP6" t="str">
         <f t="shared" si="2"/>
-        <v>000320</v>
+        <v>001410</v>
       </c>
       <c r="AQ6" t="str">
         <f t="shared" si="2"/>
-        <v>000360</v>
+        <v>001450</v>
       </c>
       <c r="AR6" t="str">
         <f t="shared" si="2"/>
-        <v>000420</v>
+        <v>001510</v>
       </c>
       <c r="AS6" t="str">
         <f t="shared" si="2"/>
-        <v>000460</v>
+        <v>001550</v>
       </c>
       <c r="AT6" t="str">
         <f t="shared" si="2"/>
-        <v>000520</v>
+        <v>001610</v>
       </c>
       <c r="AU6" t="str">
         <f t="shared" si="2"/>
-        <v>000560</v>
+        <v>001650</v>
       </c>
       <c r="AV6" t="str">
         <f t="shared" si="2"/>
-        <v>000620</v>
+        <v>001710</v>
       </c>
       <c r="AW6" t="str">
         <f t="shared" si="2"/>
-        <v>000660</v>
+        <v>001750</v>
       </c>
       <c r="AX6" t="str">
         <f t="shared" si="2"/>
-        <v>000720</v>
+        <v>002010</v>
       </c>
       <c r="AY6" t="str">
         <f t="shared" si="2"/>
-        <v>000760</v>
+        <v>002050</v>
       </c>
     </row>
     <row r="7" spans="1:51" ht="24" customHeight="1">
@@ -1275,131 +1274,131 @@
       <c r="P7" s="1"/>
       <c r="S7">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>586</v>
       </c>
       <c r="T7">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>618</v>
       </c>
       <c r="U7">
         <f t="shared" si="5"/>
-        <v>82</v>
+        <v>650</v>
       </c>
       <c r="V7">
         <f t="shared" si="6"/>
-        <v>114</v>
+        <v>682</v>
       </c>
       <c r="W7">
         <f t="shared" si="7"/>
-        <v>146</v>
+        <v>714</v>
       </c>
       <c r="X7">
         <f t="shared" si="8"/>
-        <v>178</v>
+        <v>746</v>
       </c>
       <c r="Y7">
         <f t="shared" si="9"/>
-        <v>210</v>
+        <v>778</v>
       </c>
       <c r="Z7">
         <f t="shared" si="10"/>
-        <v>242</v>
+        <v>810</v>
       </c>
       <c r="AA7">
         <f t="shared" si="11"/>
-        <v>274</v>
+        <v>842</v>
       </c>
       <c r="AB7">
         <f t="shared" si="12"/>
-        <v>306</v>
+        <v>874</v>
       </c>
       <c r="AC7">
         <f t="shared" si="13"/>
-        <v>338</v>
+        <v>906</v>
       </c>
       <c r="AD7">
         <f t="shared" si="14"/>
-        <v>370</v>
+        <v>938</v>
       </c>
       <c r="AE7">
         <f t="shared" si="15"/>
-        <v>402</v>
+        <v>970</v>
       </c>
       <c r="AF7">
         <f t="shared" si="16"/>
-        <v>434</v>
+        <v>1002</v>
       </c>
       <c r="AG7">
         <f t="shared" si="17"/>
-        <v>466</v>
+        <v>1034</v>
       </c>
       <c r="AH7">
         <f t="shared" si="18"/>
-        <v>498</v>
+        <v>1066</v>
       </c>
       <c r="AJ7" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000022</v>
+        <v>001112</v>
       </c>
       <c r="AK7" t="str">
         <f t="shared" si="19"/>
-        <v>000062</v>
+        <v>001152</v>
       </c>
       <c r="AL7" t="str">
         <f t="shared" si="19"/>
-        <v>000122</v>
+        <v>001212</v>
       </c>
       <c r="AM7" t="str">
         <f t="shared" si="2"/>
-        <v>000162</v>
+        <v>001252</v>
       </c>
       <c r="AN7" t="str">
         <f t="shared" si="2"/>
-        <v>000222</v>
+        <v>001312</v>
       </c>
       <c r="AO7" t="str">
         <f t="shared" si="2"/>
-        <v>000262</v>
+        <v>001352</v>
       </c>
       <c r="AP7" t="str">
         <f t="shared" si="2"/>
-        <v>000322</v>
+        <v>001412</v>
       </c>
       <c r="AQ7" t="str">
         <f t="shared" si="2"/>
-        <v>000362</v>
+        <v>001452</v>
       </c>
       <c r="AR7" t="str">
         <f t="shared" si="2"/>
-        <v>000422</v>
+        <v>001512</v>
       </c>
       <c r="AS7" t="str">
         <f t="shared" si="2"/>
-        <v>000462</v>
+        <v>001552</v>
       </c>
       <c r="AT7" t="str">
         <f t="shared" si="2"/>
-        <v>000522</v>
+        <v>001612</v>
       </c>
       <c r="AU7" t="str">
         <f t="shared" si="2"/>
-        <v>000562</v>
+        <v>001652</v>
       </c>
       <c r="AV7" t="str">
         <f t="shared" si="2"/>
-        <v>000622</v>
+        <v>001712</v>
       </c>
       <c r="AW7" t="str">
         <f t="shared" si="2"/>
-        <v>000662</v>
+        <v>001752</v>
       </c>
       <c r="AX7" t="str">
         <f t="shared" si="2"/>
-        <v>000722</v>
+        <v>002012</v>
       </c>
       <c r="AY7" t="str">
         <f t="shared" si="2"/>
-        <v>000762</v>
+        <v>002052</v>
       </c>
     </row>
     <row r="8" spans="1:51" ht="24" customHeight="1">
@@ -1421,131 +1420,131 @@
       <c r="P8" s="1"/>
       <c r="S8">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>588</v>
       </c>
       <c r="T8">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>620</v>
       </c>
       <c r="U8">
         <f t="shared" si="5"/>
-        <v>84</v>
+        <v>652</v>
       </c>
       <c r="V8">
         <f t="shared" si="6"/>
-        <v>116</v>
+        <v>684</v>
       </c>
       <c r="W8">
         <f t="shared" si="7"/>
-        <v>148</v>
+        <v>716</v>
       </c>
       <c r="X8">
         <f t="shared" si="8"/>
-        <v>180</v>
+        <v>748</v>
       </c>
       <c r="Y8">
         <f t="shared" si="9"/>
-        <v>212</v>
+        <v>780</v>
       </c>
       <c r="Z8">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>812</v>
       </c>
       <c r="AA8">
         <f t="shared" si="11"/>
-        <v>276</v>
+        <v>844</v>
       </c>
       <c r="AB8">
         <f t="shared" si="12"/>
-        <v>308</v>
+        <v>876</v>
       </c>
       <c r="AC8">
         <f t="shared" si="13"/>
-        <v>340</v>
+        <v>908</v>
       </c>
       <c r="AD8">
         <f t="shared" si="14"/>
-        <v>372</v>
+        <v>940</v>
       </c>
       <c r="AE8">
         <f t="shared" si="15"/>
-        <v>404</v>
+        <v>972</v>
       </c>
       <c r="AF8">
         <f t="shared" si="16"/>
-        <v>436</v>
+        <v>1004</v>
       </c>
       <c r="AG8">
         <f t="shared" si="17"/>
-        <v>468</v>
+        <v>1036</v>
       </c>
       <c r="AH8">
         <f t="shared" si="18"/>
-        <v>500</v>
+        <v>1068</v>
       </c>
       <c r="AJ8" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000024</v>
+        <v>001114</v>
       </c>
       <c r="AK8" t="str">
         <f t="shared" si="19"/>
-        <v>000064</v>
+        <v>001154</v>
       </c>
       <c r="AL8" t="str">
         <f t="shared" si="19"/>
-        <v>000124</v>
+        <v>001214</v>
       </c>
       <c r="AM8" t="str">
         <f t="shared" si="2"/>
-        <v>000164</v>
+        <v>001254</v>
       </c>
       <c r="AN8" t="str">
         <f t="shared" si="2"/>
-        <v>000224</v>
+        <v>001314</v>
       </c>
       <c r="AO8" t="str">
         <f t="shared" si="2"/>
-        <v>000264</v>
+        <v>001354</v>
       </c>
       <c r="AP8" t="str">
         <f t="shared" si="2"/>
-        <v>000324</v>
+        <v>001414</v>
       </c>
       <c r="AQ8" t="str">
         <f t="shared" si="2"/>
-        <v>000364</v>
+        <v>001454</v>
       </c>
       <c r="AR8" t="str">
         <f t="shared" si="2"/>
-        <v>000424</v>
+        <v>001514</v>
       </c>
       <c r="AS8" t="str">
         <f t="shared" si="2"/>
-        <v>000464</v>
+        <v>001554</v>
       </c>
       <c r="AT8" t="str">
         <f t="shared" si="2"/>
-        <v>000524</v>
+        <v>001614</v>
       </c>
       <c r="AU8" t="str">
         <f t="shared" si="2"/>
-        <v>000564</v>
+        <v>001654</v>
       </c>
       <c r="AV8" t="str">
         <f t="shared" si="2"/>
-        <v>000624</v>
+        <v>001714</v>
       </c>
       <c r="AW8" t="str">
         <f t="shared" si="2"/>
-        <v>000664</v>
+        <v>001754</v>
       </c>
       <c r="AX8" t="str">
         <f t="shared" si="2"/>
-        <v>000724</v>
+        <v>002014</v>
       </c>
       <c r="AY8" t="str">
         <f t="shared" si="2"/>
-        <v>000764</v>
+        <v>002054</v>
       </c>
     </row>
     <row r="9" spans="1:51" ht="24" customHeight="1">
@@ -1571,131 +1570,131 @@
       <c r="P9" s="1"/>
       <c r="S9">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>590</v>
       </c>
       <c r="T9">
         <f t="shared" si="4"/>
-        <v>54</v>
+        <v>622</v>
       </c>
       <c r="U9">
         <f t="shared" si="5"/>
-        <v>86</v>
+        <v>654</v>
       </c>
       <c r="V9">
         <f t="shared" si="6"/>
-        <v>118</v>
+        <v>686</v>
       </c>
       <c r="W9">
         <f t="shared" si="7"/>
-        <v>150</v>
+        <v>718</v>
       </c>
       <c r="X9">
         <f t="shared" si="8"/>
-        <v>182</v>
+        <v>750</v>
       </c>
       <c r="Y9">
         <f t="shared" si="9"/>
-        <v>214</v>
+        <v>782</v>
       </c>
       <c r="Z9">
         <f t="shared" si="10"/>
-        <v>246</v>
+        <v>814</v>
       </c>
       <c r="AA9">
         <f t="shared" si="11"/>
-        <v>278</v>
+        <v>846</v>
       </c>
       <c r="AB9">
         <f t="shared" si="12"/>
-        <v>310</v>
+        <v>878</v>
       </c>
       <c r="AC9">
         <f t="shared" si="13"/>
-        <v>342</v>
+        <v>910</v>
       </c>
       <c r="AD9">
         <f t="shared" si="14"/>
-        <v>374</v>
+        <v>942</v>
       </c>
       <c r="AE9">
         <f t="shared" si="15"/>
-        <v>406</v>
+        <v>974</v>
       </c>
       <c r="AF9">
         <f t="shared" si="16"/>
-        <v>438</v>
+        <v>1006</v>
       </c>
       <c r="AG9">
         <f t="shared" si="17"/>
-        <v>470</v>
+        <v>1038</v>
       </c>
       <c r="AH9">
         <f t="shared" si="18"/>
-        <v>502</v>
+        <v>1070</v>
       </c>
       <c r="AJ9" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000026</v>
+        <v>001116</v>
       </c>
       <c r="AK9" t="str">
         <f t="shared" si="19"/>
-        <v>000066</v>
+        <v>001156</v>
       </c>
       <c r="AL9" t="str">
         <f t="shared" si="19"/>
-        <v>000126</v>
+        <v>001216</v>
       </c>
       <c r="AM9" t="str">
         <f t="shared" si="2"/>
-        <v>000166</v>
+        <v>001256</v>
       </c>
       <c r="AN9" t="str">
         <f t="shared" si="2"/>
-        <v>000226</v>
+        <v>001316</v>
       </c>
       <c r="AO9" t="str">
         <f t="shared" si="2"/>
-        <v>000266</v>
+        <v>001356</v>
       </c>
       <c r="AP9" t="str">
         <f t="shared" si="2"/>
-        <v>000326</v>
+        <v>001416</v>
       </c>
       <c r="AQ9" t="str">
         <f t="shared" si="2"/>
-        <v>000366</v>
+        <v>001456</v>
       </c>
       <c r="AR9" t="str">
         <f t="shared" si="2"/>
-        <v>000426</v>
+        <v>001516</v>
       </c>
       <c r="AS9" t="str">
         <f t="shared" si="2"/>
-        <v>000466</v>
+        <v>001556</v>
       </c>
       <c r="AT9" t="str">
         <f t="shared" si="2"/>
-        <v>000526</v>
+        <v>001616</v>
       </c>
       <c r="AU9" t="str">
         <f t="shared" si="2"/>
-        <v>000566</v>
+        <v>001656</v>
       </c>
       <c r="AV9" t="str">
         <f t="shared" si="2"/>
-        <v>000626</v>
+        <v>001716</v>
       </c>
       <c r="AW9" t="str">
         <f t="shared" si="2"/>
-        <v>000666</v>
+        <v>001756</v>
       </c>
       <c r="AX9" t="str">
         <f t="shared" si="2"/>
-        <v>000726</v>
+        <v>002016</v>
       </c>
       <c r="AY9" t="str">
         <f t="shared" si="2"/>
-        <v>000766</v>
+        <v>002056</v>
       </c>
     </row>
     <row r="10" spans="1:51" ht="24" customHeight="1">
@@ -1721,131 +1720,131 @@
       <c r="P10" s="2"/>
       <c r="S10">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>592</v>
       </c>
       <c r="T10">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>624</v>
       </c>
       <c r="U10">
         <f t="shared" si="5"/>
-        <v>88</v>
+        <v>656</v>
       </c>
       <c r="V10">
         <f t="shared" si="6"/>
-        <v>120</v>
+        <v>688</v>
       </c>
       <c r="W10">
         <f t="shared" si="7"/>
-        <v>152</v>
+        <v>720</v>
       </c>
       <c r="X10">
         <f t="shared" si="8"/>
-        <v>184</v>
+        <v>752</v>
       </c>
       <c r="Y10">
         <f t="shared" si="9"/>
-        <v>216</v>
+        <v>784</v>
       </c>
       <c r="Z10">
         <f t="shared" si="10"/>
-        <v>248</v>
+        <v>816</v>
       </c>
       <c r="AA10">
         <f t="shared" si="11"/>
-        <v>280</v>
+        <v>848</v>
       </c>
       <c r="AB10">
         <f t="shared" si="12"/>
-        <v>312</v>
+        <v>880</v>
       </c>
       <c r="AC10">
         <f t="shared" si="13"/>
-        <v>344</v>
+        <v>912</v>
       </c>
       <c r="AD10">
         <f t="shared" si="14"/>
-        <v>376</v>
+        <v>944</v>
       </c>
       <c r="AE10">
         <f t="shared" si="15"/>
-        <v>408</v>
+        <v>976</v>
       </c>
       <c r="AF10">
         <f t="shared" si="16"/>
-        <v>440</v>
+        <v>1008</v>
       </c>
       <c r="AG10">
         <f t="shared" si="17"/>
-        <v>472</v>
+        <v>1040</v>
       </c>
       <c r="AH10">
         <f t="shared" si="18"/>
-        <v>504</v>
+        <v>1072</v>
       </c>
       <c r="AJ10" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000030</v>
+        <v>001120</v>
       </c>
       <c r="AK10" t="str">
         <f t="shared" si="19"/>
-        <v>000070</v>
+        <v>001160</v>
       </c>
       <c r="AL10" t="str">
         <f t="shared" si="19"/>
-        <v>000130</v>
+        <v>001220</v>
       </c>
       <c r="AM10" t="str">
         <f t="shared" si="2"/>
-        <v>000170</v>
+        <v>001260</v>
       </c>
       <c r="AN10" t="str">
         <f t="shared" si="2"/>
-        <v>000230</v>
+        <v>001320</v>
       </c>
       <c r="AO10" t="str">
         <f t="shared" si="2"/>
-        <v>000270</v>
+        <v>001360</v>
       </c>
       <c r="AP10" t="str">
         <f t="shared" si="2"/>
-        <v>000330</v>
+        <v>001420</v>
       </c>
       <c r="AQ10" t="str">
         <f t="shared" si="2"/>
-        <v>000370</v>
+        <v>001460</v>
       </c>
       <c r="AR10" t="str">
         <f t="shared" si="2"/>
-        <v>000430</v>
+        <v>001520</v>
       </c>
       <c r="AS10" t="str">
         <f t="shared" si="2"/>
-        <v>000470</v>
+        <v>001560</v>
       </c>
       <c r="AT10" t="str">
         <f t="shared" si="2"/>
-        <v>000530</v>
+        <v>001620</v>
       </c>
       <c r="AU10" t="str">
         <f t="shared" si="2"/>
-        <v>000570</v>
+        <v>001660</v>
       </c>
       <c r="AV10" t="str">
         <f t="shared" si="2"/>
-        <v>000630</v>
+        <v>001720</v>
       </c>
       <c r="AW10" t="str">
         <f t="shared" si="2"/>
-        <v>000670</v>
+        <v>001760</v>
       </c>
       <c r="AX10" t="str">
         <f t="shared" si="2"/>
-        <v>000730</v>
+        <v>002020</v>
       </c>
       <c r="AY10" t="str">
         <f t="shared" si="2"/>
-        <v>000770</v>
+        <v>002060</v>
       </c>
     </row>
     <row r="11" spans="1:51" ht="24" customHeight="1">
@@ -1873,131 +1872,131 @@
       </c>
       <c r="S11">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>594</v>
       </c>
       <c r="T11">
         <f t="shared" si="4"/>
-        <v>58</v>
+        <v>626</v>
       </c>
       <c r="U11">
         <f t="shared" si="5"/>
-        <v>90</v>
+        <v>658</v>
       </c>
       <c r="V11">
         <f t="shared" si="6"/>
-        <v>122</v>
+        <v>690</v>
       </c>
       <c r="W11">
         <f t="shared" si="7"/>
-        <v>154</v>
+        <v>722</v>
       </c>
       <c r="X11">
         <f t="shared" si="8"/>
-        <v>186</v>
+        <v>754</v>
       </c>
       <c r="Y11">
         <f t="shared" si="9"/>
-        <v>218</v>
+        <v>786</v>
       </c>
       <c r="Z11">
         <f t="shared" si="10"/>
-        <v>250</v>
+        <v>818</v>
       </c>
       <c r="AA11">
         <f t="shared" si="11"/>
-        <v>282</v>
+        <v>850</v>
       </c>
       <c r="AB11">
         <f t="shared" si="12"/>
-        <v>314</v>
+        <v>882</v>
       </c>
       <c r="AC11">
         <f t="shared" si="13"/>
-        <v>346</v>
+        <v>914</v>
       </c>
       <c r="AD11">
         <f t="shared" si="14"/>
-        <v>378</v>
+        <v>946</v>
       </c>
       <c r="AE11">
         <f t="shared" si="15"/>
-        <v>410</v>
+        <v>978</v>
       </c>
       <c r="AF11">
         <f t="shared" si="16"/>
-        <v>442</v>
+        <v>1010</v>
       </c>
       <c r="AG11">
         <f t="shared" si="17"/>
-        <v>474</v>
+        <v>1042</v>
       </c>
       <c r="AH11">
         <f t="shared" si="18"/>
-        <v>506</v>
+        <v>1074</v>
       </c>
       <c r="AJ11" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000032</v>
+        <v>001122</v>
       </c>
       <c r="AK11" t="str">
         <f t="shared" si="19"/>
-        <v>000072</v>
+        <v>001162</v>
       </c>
       <c r="AL11" t="str">
         <f t="shared" si="19"/>
-        <v>000132</v>
+        <v>001222</v>
       </c>
       <c r="AM11" t="str">
         <f t="shared" si="2"/>
-        <v>000172</v>
+        <v>001262</v>
       </c>
       <c r="AN11" t="str">
         <f t="shared" si="2"/>
-        <v>000232</v>
+        <v>001322</v>
       </c>
       <c r="AO11" t="str">
         <f t="shared" si="2"/>
-        <v>000272</v>
+        <v>001362</v>
       </c>
       <c r="AP11" t="str">
         <f t="shared" si="2"/>
-        <v>000332</v>
+        <v>001422</v>
       </c>
       <c r="AQ11" t="str">
         <f t="shared" si="2"/>
-        <v>000372</v>
+        <v>001462</v>
       </c>
       <c r="AR11" t="str">
         <f t="shared" si="2"/>
-        <v>000432</v>
+        <v>001522</v>
       </c>
       <c r="AS11" t="str">
         <f t="shared" si="2"/>
-        <v>000472</v>
+        <v>001562</v>
       </c>
       <c r="AT11" t="str">
         <f t="shared" si="2"/>
-        <v>000532</v>
+        <v>001622</v>
       </c>
       <c r="AU11" t="str">
         <f t="shared" si="2"/>
-        <v>000572</v>
+        <v>001662</v>
       </c>
       <c r="AV11" t="str">
         <f t="shared" si="2"/>
-        <v>000632</v>
+        <v>001722</v>
       </c>
       <c r="AW11" t="str">
         <f t="shared" si="2"/>
-        <v>000672</v>
+        <v>001762</v>
       </c>
       <c r="AX11" t="str">
         <f t="shared" si="2"/>
-        <v>000732</v>
+        <v>002022</v>
       </c>
       <c r="AY11" t="str">
         <f t="shared" si="2"/>
-        <v>000772</v>
+        <v>002062</v>
       </c>
     </row>
     <row r="12" spans="1:51" ht="24" customHeight="1">
@@ -2023,131 +2022,131 @@
       <c r="P12" s="2"/>
       <c r="S12">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>596</v>
       </c>
       <c r="T12">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>628</v>
       </c>
       <c r="U12">
         <f t="shared" si="5"/>
-        <v>92</v>
+        <v>660</v>
       </c>
       <c r="V12">
         <f t="shared" si="6"/>
-        <v>124</v>
+        <v>692</v>
       </c>
       <c r="W12">
         <f t="shared" si="7"/>
-        <v>156</v>
+        <v>724</v>
       </c>
       <c r="X12">
         <f t="shared" si="8"/>
-        <v>188</v>
+        <v>756</v>
       </c>
       <c r="Y12">
         <f t="shared" si="9"/>
-        <v>220</v>
+        <v>788</v>
       </c>
       <c r="Z12">
         <f t="shared" si="10"/>
-        <v>252</v>
+        <v>820</v>
       </c>
       <c r="AA12">
         <f t="shared" si="11"/>
-        <v>284</v>
+        <v>852</v>
       </c>
       <c r="AB12">
         <f t="shared" si="12"/>
-        <v>316</v>
+        <v>884</v>
       </c>
       <c r="AC12">
         <f t="shared" si="13"/>
-        <v>348</v>
+        <v>916</v>
       </c>
       <c r="AD12">
         <f t="shared" si="14"/>
-        <v>380</v>
+        <v>948</v>
       </c>
       <c r="AE12">
         <f t="shared" si="15"/>
-        <v>412</v>
+        <v>980</v>
       </c>
       <c r="AF12">
         <f t="shared" si="16"/>
-        <v>444</v>
+        <v>1012</v>
       </c>
       <c r="AG12">
         <f t="shared" si="17"/>
-        <v>476</v>
+        <v>1044</v>
       </c>
       <c r="AH12">
         <f t="shared" si="18"/>
-        <v>508</v>
+        <v>1076</v>
       </c>
       <c r="AJ12" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000034</v>
+        <v>001124</v>
       </c>
       <c r="AK12" t="str">
         <f t="shared" si="19"/>
-        <v>000074</v>
+        <v>001164</v>
       </c>
       <c r="AL12" t="str">
         <f t="shared" si="19"/>
-        <v>000134</v>
+        <v>001224</v>
       </c>
       <c r="AM12" t="str">
         <f t="shared" si="2"/>
-        <v>000174</v>
+        <v>001264</v>
       </c>
       <c r="AN12" t="str">
         <f t="shared" si="2"/>
-        <v>000234</v>
+        <v>001324</v>
       </c>
       <c r="AO12" t="str">
         <f t="shared" si="2"/>
-        <v>000274</v>
+        <v>001364</v>
       </c>
       <c r="AP12" t="str">
         <f t="shared" si="2"/>
-        <v>000334</v>
+        <v>001424</v>
       </c>
       <c r="AQ12" t="str">
         <f t="shared" si="2"/>
-        <v>000374</v>
+        <v>001464</v>
       </c>
       <c r="AR12" t="str">
         <f t="shared" si="2"/>
-        <v>000434</v>
+        <v>001524</v>
       </c>
       <c r="AS12" t="str">
         <f t="shared" si="2"/>
-        <v>000474</v>
+        <v>001564</v>
       </c>
       <c r="AT12" t="str">
         <f t="shared" si="2"/>
-        <v>000534</v>
+        <v>001624</v>
       </c>
       <c r="AU12" t="str">
         <f t="shared" si="2"/>
-        <v>000574</v>
+        <v>001664</v>
       </c>
       <c r="AV12" t="str">
         <f t="shared" si="2"/>
-        <v>000634</v>
+        <v>001724</v>
       </c>
       <c r="AW12" t="str">
         <f t="shared" si="2"/>
-        <v>000674</v>
+        <v>001764</v>
       </c>
       <c r="AX12" t="str">
         <f t="shared" si="2"/>
-        <v>000734</v>
+        <v>002024</v>
       </c>
       <c r="AY12" t="str">
         <f t="shared" si="2"/>
-        <v>000774</v>
+        <v>002064</v>
       </c>
     </row>
     <row r="13" spans="1:51" ht="24" customHeight="1">
@@ -2173,131 +2172,131 @@
       <c r="P13" s="2"/>
       <c r="S13">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>598</v>
       </c>
       <c r="T13">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>630</v>
       </c>
       <c r="U13">
         <f t="shared" si="5"/>
-        <v>94</v>
+        <v>662</v>
       </c>
       <c r="V13">
         <f t="shared" si="6"/>
-        <v>126</v>
+        <v>694</v>
       </c>
       <c r="W13">
         <f t="shared" si="7"/>
-        <v>158</v>
+        <v>726</v>
       </c>
       <c r="X13">
         <f t="shared" si="8"/>
-        <v>190</v>
+        <v>758</v>
       </c>
       <c r="Y13">
         <f t="shared" si="9"/>
-        <v>222</v>
+        <v>790</v>
       </c>
       <c r="Z13">
         <f t="shared" si="10"/>
-        <v>254</v>
+        <v>822</v>
       </c>
       <c r="AA13">
         <f t="shared" si="11"/>
-        <v>286</v>
+        <v>854</v>
       </c>
       <c r="AB13">
         <f t="shared" si="12"/>
-        <v>318</v>
+        <v>886</v>
       </c>
       <c r="AC13">
         <f t="shared" si="13"/>
-        <v>350</v>
+        <v>918</v>
       </c>
       <c r="AD13">
         <f t="shared" si="14"/>
-        <v>382</v>
+        <v>950</v>
       </c>
       <c r="AE13">
         <f t="shared" si="15"/>
-        <v>414</v>
+        <v>982</v>
       </c>
       <c r="AF13">
         <f t="shared" si="16"/>
-        <v>446</v>
+        <v>1014</v>
       </c>
       <c r="AG13">
         <f t="shared" si="17"/>
-        <v>478</v>
+        <v>1046</v>
       </c>
       <c r="AH13">
         <f t="shared" si="18"/>
-        <v>510</v>
+        <v>1078</v>
       </c>
       <c r="AJ13" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000036</v>
+        <v>001126</v>
       </c>
       <c r="AK13" t="str">
         <f t="shared" si="19"/>
-        <v>000076</v>
+        <v>001166</v>
       </c>
       <c r="AL13" t="str">
         <f t="shared" si="19"/>
-        <v>000136</v>
+        <v>001226</v>
       </c>
       <c r="AM13" t="str">
         <f t="shared" si="2"/>
-        <v>000176</v>
+        <v>001266</v>
       </c>
       <c r="AN13" t="str">
         <f t="shared" si="2"/>
-        <v>000236</v>
+        <v>001326</v>
       </c>
       <c r="AO13" t="str">
         <f t="shared" si="2"/>
-        <v>000276</v>
+        <v>001366</v>
       </c>
       <c r="AP13" t="str">
         <f t="shared" si="2"/>
-        <v>000336</v>
+        <v>001426</v>
       </c>
       <c r="AQ13" t="str">
         <f t="shared" si="2"/>
-        <v>000376</v>
+        <v>001466</v>
       </c>
       <c r="AR13" t="str">
         <f t="shared" si="2"/>
-        <v>000436</v>
+        <v>001526</v>
       </c>
       <c r="AS13" t="str">
         <f t="shared" si="2"/>
-        <v>000476</v>
+        <v>001566</v>
       </c>
       <c r="AT13" t="str">
         <f t="shared" si="2"/>
-        <v>000536</v>
+        <v>001626</v>
       </c>
       <c r="AU13" t="str">
         <f t="shared" si="2"/>
-        <v>000576</v>
+        <v>001666</v>
       </c>
       <c r="AV13" t="str">
         <f t="shared" si="2"/>
-        <v>000636</v>
+        <v>001726</v>
       </c>
       <c r="AW13" t="str">
         <f t="shared" si="2"/>
-        <v>000676</v>
+        <v>001766</v>
       </c>
       <c r="AX13" t="str">
         <f t="shared" si="2"/>
-        <v>000736</v>
+        <v>002026</v>
       </c>
       <c r="AY13" t="str">
         <f t="shared" si="2"/>
-        <v>000776</v>
+        <v>002066</v>
       </c>
     </row>
     <row r="14" spans="1:51" ht="24" customHeight="1">
@@ -2327,131 +2326,131 @@
       <c r="P14" s="2"/>
       <c r="S14">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>600</v>
       </c>
       <c r="T14">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>632</v>
       </c>
       <c r="U14">
         <f t="shared" si="5"/>
-        <v>96</v>
+        <v>664</v>
       </c>
       <c r="V14">
         <f t="shared" si="6"/>
-        <v>128</v>
+        <v>696</v>
       </c>
       <c r="W14">
         <f t="shared" si="7"/>
-        <v>160</v>
+        <v>728</v>
       </c>
       <c r="X14">
         <f t="shared" si="8"/>
-        <v>192</v>
+        <v>760</v>
       </c>
       <c r="Y14">
         <f t="shared" si="9"/>
-        <v>224</v>
+        <v>792</v>
       </c>
       <c r="Z14">
         <f t="shared" si="10"/>
-        <v>256</v>
+        <v>824</v>
       </c>
       <c r="AA14">
         <f t="shared" si="11"/>
-        <v>288</v>
+        <v>856</v>
       </c>
       <c r="AB14">
         <f t="shared" si="12"/>
-        <v>320</v>
+        <v>888</v>
       </c>
       <c r="AC14">
         <f t="shared" si="13"/>
-        <v>352</v>
+        <v>920</v>
       </c>
       <c r="AD14">
         <f t="shared" si="14"/>
-        <v>384</v>
+        <v>952</v>
       </c>
       <c r="AE14">
         <f t="shared" si="15"/>
-        <v>416</v>
+        <v>984</v>
       </c>
       <c r="AF14">
         <f t="shared" si="16"/>
-        <v>448</v>
+        <v>1016</v>
       </c>
       <c r="AG14">
         <f t="shared" si="17"/>
-        <v>480</v>
+        <v>1048</v>
       </c>
       <c r="AH14">
         <f t="shared" si="18"/>
-        <v>512</v>
+        <v>1080</v>
       </c>
       <c r="AJ14" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000040</v>
+        <v>001130</v>
       </c>
       <c r="AK14" t="str">
         <f t="shared" si="19"/>
-        <v>000100</v>
+        <v>001170</v>
       </c>
       <c r="AL14" t="str">
         <f t="shared" si="19"/>
-        <v>000140</v>
+        <v>001230</v>
       </c>
       <c r="AM14" t="str">
         <f t="shared" si="2"/>
-        <v>000200</v>
+        <v>001270</v>
       </c>
       <c r="AN14" t="str">
         <f t="shared" si="2"/>
-        <v>000240</v>
+        <v>001330</v>
       </c>
       <c r="AO14" t="str">
         <f t="shared" si="2"/>
-        <v>000300</v>
+        <v>001370</v>
       </c>
       <c r="AP14" t="str">
         <f t="shared" si="2"/>
-        <v>000340</v>
+        <v>001430</v>
       </c>
       <c r="AQ14" t="str">
         <f t="shared" si="2"/>
-        <v>000400</v>
+        <v>001470</v>
       </c>
       <c r="AR14" t="str">
         <f t="shared" si="2"/>
-        <v>000440</v>
+        <v>001530</v>
       </c>
       <c r="AS14" t="str">
         <f t="shared" si="2"/>
-        <v>000500</v>
+        <v>001570</v>
       </c>
       <c r="AT14" t="str">
         <f t="shared" si="2"/>
-        <v>000540</v>
+        <v>001630</v>
       </c>
       <c r="AU14" t="str">
         <f t="shared" si="2"/>
-        <v>000600</v>
+        <v>001670</v>
       </c>
       <c r="AV14" t="str">
         <f t="shared" si="2"/>
-        <v>000640</v>
+        <v>001730</v>
       </c>
       <c r="AW14" t="str">
         <f t="shared" si="2"/>
-        <v>000700</v>
+        <v>001770</v>
       </c>
       <c r="AX14" t="str">
         <f t="shared" si="2"/>
-        <v>000740</v>
+        <v>002030</v>
       </c>
       <c r="AY14" t="str">
         <f t="shared" si="2"/>
-        <v>001000</v>
+        <v>002070</v>
       </c>
     </row>
     <row r="15" spans="1:51" ht="24" customHeight="1">
@@ -2479,131 +2478,131 @@
       <c r="P15" s="2"/>
       <c r="S15">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>602</v>
       </c>
       <c r="T15">
         <f t="shared" si="4"/>
-        <v>66</v>
+        <v>634</v>
       </c>
       <c r="U15">
         <f t="shared" si="5"/>
-        <v>98</v>
+        <v>666</v>
       </c>
       <c r="V15">
         <f t="shared" si="6"/>
-        <v>130</v>
+        <v>698</v>
       </c>
       <c r="W15">
         <f t="shared" si="7"/>
-        <v>162</v>
+        <v>730</v>
       </c>
       <c r="X15">
         <f t="shared" si="8"/>
-        <v>194</v>
+        <v>762</v>
       </c>
       <c r="Y15">
         <f t="shared" si="9"/>
-        <v>226</v>
+        <v>794</v>
       </c>
       <c r="Z15">
         <f t="shared" si="10"/>
-        <v>258</v>
+        <v>826</v>
       </c>
       <c r="AA15">
         <f t="shared" si="11"/>
-        <v>290</v>
+        <v>858</v>
       </c>
       <c r="AB15">
         <f t="shared" si="12"/>
-        <v>322</v>
+        <v>890</v>
       </c>
       <c r="AC15">
         <f t="shared" si="13"/>
-        <v>354</v>
+        <v>922</v>
       </c>
       <c r="AD15">
         <f t="shared" si="14"/>
-        <v>386</v>
+        <v>954</v>
       </c>
       <c r="AE15">
         <f t="shared" si="15"/>
-        <v>418</v>
+        <v>986</v>
       </c>
       <c r="AF15">
         <f t="shared" si="16"/>
-        <v>450</v>
+        <v>1018</v>
       </c>
       <c r="AG15">
         <f t="shared" si="17"/>
-        <v>482</v>
+        <v>1050</v>
       </c>
       <c r="AH15">
         <f t="shared" si="18"/>
-        <v>514</v>
+        <v>1082</v>
       </c>
       <c r="AJ15" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000042</v>
+        <v>001132</v>
       </c>
       <c r="AK15" t="str">
         <f t="shared" si="19"/>
-        <v>000102</v>
+        <v>001172</v>
       </c>
       <c r="AL15" t="str">
         <f t="shared" si="19"/>
-        <v>000142</v>
+        <v>001232</v>
       </c>
       <c r="AM15" t="str">
         <f t="shared" si="2"/>
-        <v>000202</v>
+        <v>001272</v>
       </c>
       <c r="AN15" t="str">
         <f t="shared" si="2"/>
-        <v>000242</v>
+        <v>001332</v>
       </c>
       <c r="AO15" t="str">
         <f t="shared" si="2"/>
-        <v>000302</v>
+        <v>001372</v>
       </c>
       <c r="AP15" t="str">
         <f t="shared" si="2"/>
-        <v>000342</v>
+        <v>001432</v>
       </c>
       <c r="AQ15" t="str">
         <f t="shared" si="2"/>
-        <v>000402</v>
+        <v>001472</v>
       </c>
       <c r="AR15" t="str">
         <f t="shared" si="2"/>
-        <v>000442</v>
+        <v>001532</v>
       </c>
       <c r="AS15" t="str">
         <f t="shared" si="2"/>
-        <v>000502</v>
+        <v>001572</v>
       </c>
       <c r="AT15" t="str">
         <f t="shared" si="2"/>
-        <v>000542</v>
+        <v>001632</v>
       </c>
       <c r="AU15" t="str">
         <f t="shared" si="2"/>
-        <v>000602</v>
+        <v>001672</v>
       </c>
       <c r="AV15" t="str">
         <f t="shared" si="2"/>
-        <v>000642</v>
+        <v>001732</v>
       </c>
       <c r="AW15" t="str">
         <f t="shared" si="2"/>
-        <v>000702</v>
+        <v>001772</v>
       </c>
       <c r="AX15" t="str">
         <f t="shared" si="2"/>
-        <v>000742</v>
+        <v>002032</v>
       </c>
       <c r="AY15" t="str">
         <f t="shared" si="2"/>
-        <v>001002</v>
+        <v>002072</v>
       </c>
     </row>
     <row r="16" spans="1:51" ht="24" customHeight="1">
@@ -2629,131 +2628,131 @@
       <c r="P16" s="2"/>
       <c r="S16">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>604</v>
       </c>
       <c r="T16">
         <f t="shared" si="4"/>
-        <v>68</v>
+        <v>636</v>
       </c>
       <c r="U16">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>668</v>
       </c>
       <c r="V16">
         <f t="shared" si="6"/>
-        <v>132</v>
+        <v>700</v>
       </c>
       <c r="W16">
         <f t="shared" si="7"/>
-        <v>164</v>
+        <v>732</v>
       </c>
       <c r="X16">
         <f t="shared" si="8"/>
-        <v>196</v>
+        <v>764</v>
       </c>
       <c r="Y16">
         <f t="shared" si="9"/>
-        <v>228</v>
+        <v>796</v>
       </c>
       <c r="Z16">
         <f t="shared" si="10"/>
-        <v>260</v>
+        <v>828</v>
       </c>
       <c r="AA16">
         <f t="shared" si="11"/>
-        <v>292</v>
+        <v>860</v>
       </c>
       <c r="AB16">
         <f t="shared" si="12"/>
-        <v>324</v>
+        <v>892</v>
       </c>
       <c r="AC16">
         <f t="shared" si="13"/>
-        <v>356</v>
+        <v>924</v>
       </c>
       <c r="AD16">
         <f t="shared" si="14"/>
-        <v>388</v>
+        <v>956</v>
       </c>
       <c r="AE16">
         <f t="shared" si="15"/>
-        <v>420</v>
+        <v>988</v>
       </c>
       <c r="AF16">
         <f t="shared" si="16"/>
-        <v>452</v>
+        <v>1020</v>
       </c>
       <c r="AG16">
         <f t="shared" si="17"/>
-        <v>484</v>
+        <v>1052</v>
       </c>
       <c r="AH16">
         <f t="shared" si="18"/>
-        <v>516</v>
+        <v>1084</v>
       </c>
       <c r="AJ16" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000044</v>
+        <v>001134</v>
       </c>
       <c r="AK16" t="str">
         <f t="shared" si="19"/>
-        <v>000104</v>
+        <v>001174</v>
       </c>
       <c r="AL16" t="str">
         <f t="shared" si="19"/>
-        <v>000144</v>
+        <v>001234</v>
       </c>
       <c r="AM16" t="str">
         <f t="shared" si="2"/>
-        <v>000204</v>
+        <v>001274</v>
       </c>
       <c r="AN16" t="str">
         <f t="shared" si="2"/>
-        <v>000244</v>
+        <v>001334</v>
       </c>
       <c r="AO16" t="str">
         <f t="shared" si="2"/>
-        <v>000304</v>
+        <v>001374</v>
       </c>
       <c r="AP16" t="str">
         <f t="shared" si="2"/>
-        <v>000344</v>
+        <v>001434</v>
       </c>
       <c r="AQ16" t="str">
         <f t="shared" si="2"/>
-        <v>000404</v>
+        <v>001474</v>
       </c>
       <c r="AR16" t="str">
         <f t="shared" si="2"/>
-        <v>000444</v>
+        <v>001534</v>
       </c>
       <c r="AS16" t="str">
         <f t="shared" si="2"/>
-        <v>000504</v>
+        <v>001574</v>
       </c>
       <c r="AT16" t="str">
         <f t="shared" si="2"/>
-        <v>000544</v>
+        <v>001634</v>
       </c>
       <c r="AU16" t="str">
         <f t="shared" si="2"/>
-        <v>000604</v>
+        <v>001674</v>
       </c>
       <c r="AV16" t="str">
         <f t="shared" si="2"/>
-        <v>000644</v>
+        <v>001734</v>
       </c>
       <c r="AW16" t="str">
         <f t="shared" si="2"/>
-        <v>000704</v>
+        <v>001774</v>
       </c>
       <c r="AX16" t="str">
         <f t="shared" si="2"/>
-        <v>000744</v>
+        <v>002034</v>
       </c>
       <c r="AY16" t="str">
         <f t="shared" si="2"/>
-        <v>001004</v>
+        <v>002074</v>
       </c>
     </row>
     <row r="17" spans="1:51" ht="24" customHeight="1">
@@ -2775,131 +2774,131 @@
       <c r="P17" s="2"/>
       <c r="S17">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>606</v>
       </c>
       <c r="T17">
         <f t="shared" si="4"/>
-        <v>70</v>
+        <v>638</v>
       </c>
       <c r="U17">
         <f t="shared" si="5"/>
-        <v>102</v>
+        <v>670</v>
       </c>
       <c r="V17">
         <f t="shared" si="6"/>
-        <v>134</v>
+        <v>702</v>
       </c>
       <c r="W17">
         <f t="shared" si="7"/>
-        <v>166</v>
+        <v>734</v>
       </c>
       <c r="X17">
         <f t="shared" si="8"/>
-        <v>198</v>
+        <v>766</v>
       </c>
       <c r="Y17">
         <f t="shared" si="9"/>
-        <v>230</v>
+        <v>798</v>
       </c>
       <c r="Z17">
         <f t="shared" si="10"/>
-        <v>262</v>
+        <v>830</v>
       </c>
       <c r="AA17">
         <f t="shared" si="11"/>
-        <v>294</v>
+        <v>862</v>
       </c>
       <c r="AB17">
         <f t="shared" si="12"/>
-        <v>326</v>
+        <v>894</v>
       </c>
       <c r="AC17">
         <f t="shared" si="13"/>
-        <v>358</v>
+        <v>926</v>
       </c>
       <c r="AD17">
         <f t="shared" si="14"/>
-        <v>390</v>
+        <v>958</v>
       </c>
       <c r="AE17">
         <f t="shared" si="15"/>
-        <v>422</v>
+        <v>990</v>
       </c>
       <c r="AF17">
         <f t="shared" si="16"/>
-        <v>454</v>
+        <v>1022</v>
       </c>
       <c r="AG17">
         <f t="shared" si="17"/>
-        <v>486</v>
+        <v>1054</v>
       </c>
       <c r="AH17">
         <f t="shared" si="18"/>
-        <v>518</v>
+        <v>1086</v>
       </c>
       <c r="AJ17" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>000046</v>
+        <v>001136</v>
       </c>
       <c r="AK17" t="str">
         <f t="shared" si="19"/>
-        <v>000106</v>
+        <v>001176</v>
       </c>
       <c r="AL17" t="str">
         <f t="shared" si="19"/>
-        <v>000146</v>
+        <v>001236</v>
       </c>
       <c r="AM17" t="str">
         <f t="shared" si="2"/>
-        <v>000206</v>
+        <v>001276</v>
       </c>
       <c r="AN17" t="str">
         <f t="shared" si="2"/>
-        <v>000246</v>
+        <v>001336</v>
       </c>
       <c r="AO17" t="str">
         <f t="shared" si="2"/>
-        <v>000306</v>
+        <v>001376</v>
       </c>
       <c r="AP17" t="str">
         <f t="shared" si="2"/>
-        <v>000346</v>
+        <v>001436</v>
       </c>
       <c r="AQ17" t="str">
         <f t="shared" si="2"/>
-        <v>000406</v>
+        <v>001476</v>
       </c>
       <c r="AR17" t="str">
         <f t="shared" si="2"/>
-        <v>000446</v>
+        <v>001536</v>
       </c>
       <c r="AS17" t="str">
         <f t="shared" si="2"/>
-        <v>000506</v>
+        <v>001576</v>
       </c>
       <c r="AT17" t="str">
         <f t="shared" si="2"/>
-        <v>000546</v>
+        <v>001636</v>
       </c>
       <c r="AU17" t="str">
         <f t="shared" si="2"/>
-        <v>000606</v>
+        <v>001676</v>
       </c>
       <c r="AV17" t="str">
         <f t="shared" si="2"/>
-        <v>000646</v>
+        <v>001736</v>
       </c>
       <c r="AW17" t="str">
         <f t="shared" si="2"/>
-        <v>000706</v>
+        <v>001776</v>
       </c>
       <c r="AX17" t="str">
         <f t="shared" si="2"/>
-        <v>000746</v>
+        <v>002036</v>
       </c>
       <c r="AY17" t="str">
         <f t="shared" si="2"/>
-        <v>001006</v>
+        <v>002076</v>
       </c>
     </row>
     <row r="18" spans="1:51">

</xml_diff>